<commit_message>
corretto esercizio 1.16.2.3 programmazione laboratorio
</commit_message>
<xml_diff>
--- a/Bruniera/laboratorio programmazione/esercizi/java/1.16.1/1.16.1.3.xlsx
+++ b/Bruniera/laboratorio programmazione/esercizi/java/1.16.1/1.16.1.3.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C55F88-7BDF-41A0-86B7-C0ADD0B8A6F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05573E4F-7EFF-4030-B768-2C7CC372C7E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,11 +472,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Cella collegata" xfId="2" builtinId="24"/>
@@ -761,18 +762,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:A87"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -785,7 +787,7 @@
       <c r="C1">
         <v>337</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="4">
         <v>1111</v>
       </c>
       <c r="E1">
@@ -804,7 +806,7 @@
       <c r="N1">
         <v>82</v>
       </c>
-      <c r="O1">
+      <c r="O1" s="4">
         <v>100000</v>
       </c>
       <c r="P1">
@@ -825,7 +827,7 @@
       <c r="C2">
         <v>337</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>1110</v>
       </c>
       <c r="E2">
@@ -844,7 +846,7 @@
       <c r="N2">
         <v>97</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="4">
         <v>1100001</v>
       </c>
       <c r="P2">
@@ -865,7 +867,7 @@
       <c r="C3">
         <v>3663</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>11</v>
       </c>
       <c r="E3">
@@ -884,7 +886,7 @@
       <c r="N3">
         <v>84</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="4">
         <v>101001</v>
       </c>
       <c r="P3">
@@ -905,7 +907,7 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>1000011011</v>
       </c>
       <c r="E4">
@@ -924,7 +926,7 @@
       <c r="N4">
         <v>81</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>11111</v>
       </c>
       <c r="P4">
@@ -945,7 +947,7 @@
       <c r="C5">
         <v>56</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
       <c r="E5">
@@ -964,7 +966,7 @@
       <c r="N5">
         <v>97</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="4">
         <v>1100110</v>
       </c>
       <c r="P5">
@@ -985,7 +987,7 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>10000011100110</v>
       </c>
       <c r="E6">
@@ -1004,7 +1006,7 @@
       <c r="N6">
         <v>89</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="4">
         <v>1000000</v>
       </c>
       <c r="P6">
@@ -1025,7 +1027,7 @@
       <c r="C7">
         <v>50</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>10011011</v>
       </c>
       <c r="E7">
@@ -1044,7 +1046,7 @@
       <c r="N7">
         <v>83</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="4">
         <v>100100</v>
       </c>
       <c r="P7">
@@ -1065,7 +1067,7 @@
       <c r="C8">
         <v>136</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>10000</v>
       </c>
       <c r="E8">
@@ -1084,7 +1086,7 @@
       <c r="N8">
         <v>73</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="4">
         <v>1100</v>
       </c>
       <c r="P8">
@@ -1105,7 +1107,7 @@
       <c r="C9">
         <v>136</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>10001</v>
       </c>
       <c r="E9">
@@ -1124,7 +1126,7 @@
       <c r="N9">
         <v>89</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="4">
         <v>111110</v>
       </c>
       <c r="P9">
@@ -1145,7 +1147,7 @@
       <c r="C10">
         <v>11</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>1000001111</v>
       </c>
       <c r="E10">
@@ -1164,7 +1166,7 @@
       <c r="N10">
         <v>92</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="4">
         <v>1010000</v>
       </c>
       <c r="P10">
@@ -1185,7 +1187,7 @@
       <c r="C11">
         <v>29</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>111</v>
       </c>
       <c r="E11">
@@ -1204,7 +1206,7 @@
       <c r="N11">
         <v>88</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="4">
         <v>110111</v>
       </c>
       <c r="P11">
@@ -1225,7 +1227,7 @@
       <c r="C12">
         <v>23</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>100110010</v>
       </c>
       <c r="E12">
@@ -1244,7 +1246,7 @@
       <c r="N12">
         <v>89</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="4">
         <v>111010</v>
       </c>
       <c r="P12">
@@ -1265,7 +1267,7 @@
       <c r="C13">
         <v>76</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>101101</v>
       </c>
       <c r="E13">
@@ -1284,7 +1286,7 @@
       <c r="N13">
         <v>87</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="4">
         <v>110011</v>
       </c>
       <c r="P13">
@@ -1305,7 +1307,7 @@
       <c r="C14">
         <v>106</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>1001111</v>
       </c>
       <c r="E14">
@@ -1324,7 +1326,7 @@
       <c r="N14">
         <v>97</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="4">
         <v>1100100</v>
       </c>
       <c r="P14">
@@ -1345,7 +1347,7 @@
       <c r="C15">
         <v>420</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>10101</v>
       </c>
       <c r="E15">
@@ -1364,7 +1366,7 @@
       <c r="N15">
         <v>71</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="4">
         <v>110</v>
       </c>
       <c r="P15">
@@ -1385,7 +1387,7 @@
       <c r="C16">
         <v>20</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>100000110</v>
       </c>
       <c r="E16">
@@ -1404,7 +1406,7 @@
       <c r="N16">
         <v>91</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="4">
         <v>1001000</v>
       </c>
       <c r="P16">
@@ -1425,7 +1427,7 @@
       <c r="C17">
         <v>18</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>10011100</v>
       </c>
       <c r="E17">
@@ -1444,7 +1446,7 @@
       <c r="N17">
         <v>94</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="4">
         <v>1010111</v>
       </c>
       <c r="P17">
@@ -1465,7 +1467,7 @@
       <c r="C18">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>10011010110</v>
       </c>
       <c r="E18">
@@ -1484,7 +1486,7 @@
       <c r="N18">
         <v>96</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="4">
         <v>1011111</v>
       </c>
       <c r="P18">
@@ -1505,7 +1507,7 @@
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>10011000101</v>
       </c>
       <c r="E19">
@@ -1524,7 +1526,7 @@
       <c r="N19">
         <v>98</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="4">
         <v>1101001</v>
       </c>
       <c r="P19">
@@ -1545,7 +1547,7 @@
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>10011000110</v>
       </c>
       <c r="E20">
@@ -1564,7 +1566,7 @@
       <c r="N20">
         <v>77</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="4">
         <v>10001</v>
       </c>
       <c r="P20">
@@ -1585,7 +1587,7 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>10000011100111</v>
       </c>
       <c r="E21">
@@ -1604,7 +1606,7 @@
       <c r="N21">
         <v>97</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="4">
         <v>1100010</v>
       </c>
       <c r="P21">
@@ -1625,7 +1627,7 @@
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>1000011001</v>
       </c>
       <c r="E22">
@@ -1644,7 +1646,7 @@
       <c r="N22">
         <v>87</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="4">
         <v>110101</v>
       </c>
       <c r="P22">
@@ -1665,7 +1667,7 @@
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>100110100001</v>
       </c>
       <c r="E23">
@@ -1684,7 +1686,7 @@
       <c r="N23">
         <v>106</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="4">
         <v>1111000</v>
       </c>
       <c r="P23">
@@ -1705,7 +1707,7 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>100110001000</v>
       </c>
       <c r="E24">
@@ -1724,7 +1726,7 @@
       <c r="N24">
         <v>90</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="4">
         <v>1000110</v>
       </c>
       <c r="P24">
@@ -1745,7 +1747,7 @@
       <c r="C25">
         <v>44</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>10011000</v>
       </c>
       <c r="E25">
@@ -1764,7 +1766,7 @@
       <c r="N25">
         <v>107</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="4">
         <v>1111001</v>
       </c>
       <c r="P25">
@@ -1785,7 +1787,7 @@
       <c r="C26">
         <v>106</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>1001110</v>
       </c>
       <c r="E26">
@@ -1804,7 +1806,7 @@
       <c r="N26">
         <v>77</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="4">
         <v>10010</v>
       </c>
       <c r="P26">
@@ -1825,7 +1827,7 @@
       <c r="C27">
         <v>12</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>1001101010</v>
       </c>
       <c r="E27">
@@ -1844,7 +1846,7 @@
       <c r="N27">
         <v>100</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="4">
         <v>1101101</v>
       </c>
       <c r="P27">
@@ -1865,7 +1867,7 @@
       <c r="C28">
         <v>66</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>10011</v>
       </c>
       <c r="E28">
@@ -1884,7 +1886,7 @@
       <c r="N28">
         <v>97</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="4">
         <v>1100011</v>
       </c>
       <c r="P28">
@@ -1905,7 +1907,7 @@
       <c r="C29">
         <v>9</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>100110011</v>
       </c>
       <c r="E29">
@@ -1924,7 +1926,7 @@
       <c r="N29">
         <v>94</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="4">
         <v>1011011</v>
       </c>
       <c r="P29">
@@ -1945,7 +1947,7 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <v>1000001110010</v>
       </c>
       <c r="E30">
@@ -1964,7 +1966,7 @@
       <c r="N30">
         <v>93</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="4">
         <v>1010101</v>
       </c>
       <c r="P30">
@@ -1985,7 +1987,7 @@
       <c r="C31">
         <v>9</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <v>100111110</v>
       </c>
       <c r="E31">
@@ -2004,7 +2006,7 @@
       <c r="N31">
         <v>108</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="4">
         <v>1111011</v>
       </c>
       <c r="P31">
@@ -2025,7 +2027,7 @@
       <c r="C32">
         <v>8</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>100110000</v>
       </c>
       <c r="E32">
@@ -2044,7 +2046,7 @@
       <c r="N32">
         <v>88</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="4">
         <v>110110</v>
       </c>
       <c r="P32">
@@ -2065,7 +2067,7 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>1000001110000</v>
       </c>
       <c r="E33">
@@ -2084,7 +2086,7 @@
       <c r="N33">
         <v>90</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="4">
         <v>1000001</v>
       </c>
       <c r="P33">
@@ -2105,7 +2107,7 @@
       <c r="C34">
         <v>27</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34">
@@ -2124,7 +2126,7 @@
       <c r="N34">
         <v>84</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="4">
         <v>100111</v>
       </c>
       <c r="P34">
@@ -2145,7 +2147,7 @@
       <c r="C35">
         <v>5</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="4">
         <v>10000011101</v>
       </c>
       <c r="E35">
@@ -2164,7 +2166,7 @@
       <c r="N35">
         <v>71</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="4">
         <v>111</v>
       </c>
       <c r="P35">
@@ -2185,7 +2187,7 @@
       <c r="C36">
         <v>1</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <v>1000001110001</v>
       </c>
       <c r="E36">
@@ -2204,7 +2206,7 @@
       <c r="N36">
         <v>81</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="4">
         <v>11110</v>
       </c>
       <c r="P36">
@@ -2225,7 +2227,7 @@
       <c r="C37">
         <v>19</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="4">
         <v>10011110</v>
       </c>
       <c r="E37">
@@ -2244,7 +2246,7 @@
       <c r="N37">
         <v>84</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="4">
         <v>101000</v>
       </c>
       <c r="P37">
@@ -2265,7 +2267,7 @@
       <c r="C38">
         <v>31</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="4">
         <v>1011</v>
       </c>
       <c r="E38">
@@ -2284,7 +2286,7 @@
       <c r="N38">
         <v>74</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="4">
         <v>1101</v>
       </c>
       <c r="P38">
@@ -2305,7 +2307,7 @@
       <c r="C39">
         <v>15</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="4">
         <v>1000010</v>
       </c>
       <c r="E39">
@@ -2324,7 +2326,7 @@
       <c r="N39">
         <v>104</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="4">
         <v>1110011</v>
       </c>
       <c r="P39">
@@ -2345,7 +2347,7 @@
       <c r="C40">
         <v>8</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="4">
         <v>10000111</v>
       </c>
       <c r="E40">
@@ -2364,7 +2366,7 @@
       <c r="N40">
         <v>84</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="4">
         <v>101010</v>
       </c>
       <c r="P40">
@@ -2385,7 +2387,7 @@
       <c r="C41">
         <v>2</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="4">
         <v>10011000111</v>
       </c>
       <c r="E41">
@@ -2404,7 +2406,7 @@
       <c r="N41">
         <v>94</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="4">
         <v>1011000</v>
       </c>
       <c r="P41">
@@ -2425,7 +2427,7 @@
       <c r="C42">
         <v>24</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="4">
         <v>100110011</v>
       </c>
       <c r="E42">
@@ -2444,7 +2446,7 @@
       <c r="N42">
         <v>89</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="4">
         <v>111111</v>
       </c>
       <c r="P42">
@@ -2465,7 +2467,7 @@
       <c r="C43">
         <v>8</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="4">
         <v>100110010</v>
       </c>
       <c r="E43">
@@ -2484,7 +2486,7 @@
       <c r="N43">
         <v>80</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="4">
         <v>11000</v>
       </c>
       <c r="P43">
@@ -2505,7 +2507,7 @@
       <c r="C44">
         <v>3</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="4">
         <v>100110100000</v>
       </c>
       <c r="E44">
@@ -2524,7 +2526,7 @@
       <c r="N44">
         <v>105</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="4">
         <v>1110101</v>
       </c>
       <c r="P44">
@@ -2545,7 +2547,7 @@
       <c r="C45">
         <v>2</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="4">
         <v>1000011010</v>
       </c>
       <c r="E45">
@@ -2564,7 +2566,7 @@
       <c r="N45">
         <v>93</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="4">
         <v>1010011</v>
       </c>
       <c r="P45">
@@ -2585,7 +2587,7 @@
       <c r="C46">
         <v>7</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="4">
         <v>10011010111</v>
       </c>
       <c r="E46">
@@ -2604,7 +2606,7 @@
       <c r="N46">
         <v>76</v>
       </c>
-      <c r="O46">
+      <c r="O46" s="4">
         <v>10000</v>
       </c>
       <c r="P46">
@@ -2625,7 +2627,7 @@
       <c r="C47">
         <v>36</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="4">
         <v>1001101</v>
       </c>
       <c r="E47">
@@ -2644,7 +2646,7 @@
       <c r="N47">
         <v>89</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="4">
         <v>111100</v>
       </c>
       <c r="P47">
@@ -2665,7 +2667,7 @@
       <c r="C48">
         <v>41</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="4">
         <v>10000010</v>
       </c>
       <c r="E48">
@@ -2684,7 +2686,7 @@
       <c r="N48">
         <v>101</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="4">
         <v>1110000</v>
       </c>
       <c r="P48">
@@ -2705,7 +2707,7 @@
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="4">
         <v>100110001001</v>
       </c>
       <c r="E49">
@@ -2724,7 +2726,7 @@
       <c r="N49">
         <v>90</v>
       </c>
-      <c r="O49">
+      <c r="O49" s="4">
         <v>1000111</v>
       </c>
       <c r="P49">
@@ -2745,7 +2747,7 @@
       <c r="C50">
         <v>30</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="4">
         <v>1001</v>
       </c>
       <c r="E50">
@@ -2764,7 +2766,7 @@
       <c r="N50">
         <v>94</v>
       </c>
-      <c r="O50">
+      <c r="O50" s="4">
         <v>1011010</v>
       </c>
       <c r="P50">
@@ -2785,7 +2787,7 @@
       <c r="C51">
         <v>18</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="4">
         <v>10011101</v>
       </c>
       <c r="E51">
@@ -2804,7 +2806,7 @@
       <c r="N51">
         <v>88</v>
       </c>
-      <c r="O51">
+      <c r="O51" s="4">
         <v>111000</v>
       </c>
       <c r="P51">
@@ -2825,7 +2827,7 @@
       <c r="C52">
         <v>30</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="4">
         <v>1010</v>
       </c>
       <c r="E52">
@@ -2844,7 +2846,7 @@
       <c r="N52">
         <v>89</v>
       </c>
-      <c r="O52">
+      <c r="O52" s="4">
         <v>111011</v>
       </c>
       <c r="P52">
@@ -2865,7 +2867,7 @@
       <c r="C53">
         <v>6</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="4">
         <v>10011010001</v>
       </c>
       <c r="E53">
@@ -2884,7 +2886,7 @@
       <c r="N53">
         <v>80</v>
       </c>
-      <c r="O53">
+      <c r="O53" s="4">
         <v>11010</v>
       </c>
       <c r="P53">
@@ -2905,7 +2907,7 @@
       <c r="C54">
         <v>389</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="4">
         <v>10010</v>
       </c>
       <c r="E54">
@@ -2924,7 +2926,7 @@
       <c r="N54">
         <v>91</v>
       </c>
-      <c r="O54">
+      <c r="O54" s="4">
         <v>1001101</v>
       </c>
       <c r="P54">
@@ -2945,7 +2947,7 @@
       <c r="C55">
         <v>58</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="4">
         <v>10</v>
       </c>
       <c r="E55">
@@ -2964,7 +2966,7 @@
       <c r="N55">
         <v>93</v>
       </c>
-      <c r="O55">
+      <c r="O55" s="4">
         <v>1010110</v>
       </c>
       <c r="P55">
@@ -2985,7 +2987,7 @@
       <c r="C56">
         <v>306</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="4">
         <v>1010</v>
       </c>
       <c r="E56">
@@ -3004,7 +3006,7 @@
       <c r="N56">
         <v>80</v>
       </c>
-      <c r="O56">
+      <c r="O56" s="4">
         <v>10111</v>
       </c>
       <c r="P56">
@@ -3025,7 +3027,7 @@
       <c r="C57">
         <v>262</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="4">
         <v>110</v>
       </c>
       <c r="E57">
@@ -3044,7 +3046,7 @@
       <c r="N57">
         <v>91</v>
       </c>
-      <c r="O57">
+      <c r="O57" s="4">
         <v>1001110</v>
       </c>
       <c r="P57">
@@ -3065,7 +3067,7 @@
       <c r="C58">
         <v>621</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="4">
         <v>110</v>
       </c>
       <c r="E58">
@@ -3084,7 +3086,7 @@
       <c r="N58">
         <v>104</v>
       </c>
-      <c r="O58">
+      <c r="O58" s="4">
         <v>1110010</v>
       </c>
       <c r="P58">
@@ -3105,7 +3107,7 @@
       <c r="C59">
         <v>157</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="4">
         <v>10111</v>
       </c>
       <c r="E59">
@@ -3124,7 +3126,7 @@
       <c r="N59">
         <v>87</v>
       </c>
-      <c r="O59">
+      <c r="O59" s="4">
         <v>110000</v>
       </c>
       <c r="P59">
@@ -3145,7 +3147,7 @@
       <c r="C60">
         <v>75</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="4">
         <v>101100</v>
       </c>
       <c r="E60">
@@ -3164,7 +3166,7 @@
       <c r="N60">
         <v>96</v>
       </c>
-      <c r="O60">
+      <c r="O60" s="4">
         <v>1011110</v>
       </c>
       <c r="P60">
@@ -3185,7 +3187,7 @@
       <c r="C61">
         <v>64</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="4">
         <v>10001</v>
       </c>
       <c r="E61">
@@ -3204,7 +3206,7 @@
       <c r="N61">
         <v>81</v>
       </c>
-      <c r="O61">
+      <c r="O61" s="4">
         <v>11101</v>
       </c>
       <c r="P61">
@@ -3225,7 +3227,7 @@
       <c r="C62">
         <v>479</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="4">
         <v>1</v>
       </c>
       <c r="E62">
@@ -3244,7 +3246,7 @@
       <c r="N62">
         <v>107</v>
       </c>
-      <c r="O62">
+      <c r="O62" s="4">
         <v>1111010</v>
       </c>
       <c r="P62">
@@ -3265,7 +3267,7 @@
       <c r="C63">
         <v>33</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="4">
         <v>100101</v>
       </c>
       <c r="E63">
@@ -3284,7 +3286,7 @@
       <c r="N63">
         <v>83</v>
       </c>
-      <c r="O63">
+      <c r="O63" s="4">
         <v>100110</v>
       </c>
       <c r="P63">
@@ -3305,7 +3307,7 @@
       <c r="C64">
         <v>10</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="4">
         <v>100111111</v>
       </c>
       <c r="E64">
@@ -3324,7 +3326,7 @@
       <c r="N64">
         <v>91</v>
       </c>
-      <c r="O64">
+      <c r="O64" s="4">
         <v>1001011</v>
       </c>
       <c r="P64">
@@ -3345,7 +3347,7 @@
       <c r="C65">
         <v>258</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="4">
         <v>101</v>
       </c>
       <c r="E65">
@@ -3364,7 +3366,7 @@
       <c r="N65">
         <v>105</v>
       </c>
-      <c r="O65">
+      <c r="O65" s="4">
         <v>1110100</v>
       </c>
       <c r="P65">
@@ -3385,7 +3387,7 @@
       <c r="C66">
         <v>142</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="4">
         <v>10010</v>
       </c>
       <c r="E66">
@@ -3404,7 +3406,7 @@
       <c r="N66">
         <v>102</v>
       </c>
-      <c r="O66">
+      <c r="O66" s="4">
         <v>1110001</v>
       </c>
       <c r="P66">
@@ -3425,7 +3427,7 @@
       <c r="C67">
         <v>353</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="4">
         <v>10001</v>
       </c>
       <c r="E67">
@@ -3444,7 +3446,7 @@
       <c r="N67">
         <v>74</v>
       </c>
-      <c r="O67">
+      <c r="O67" s="4">
         <v>1110</v>
       </c>
       <c r="P67">
@@ -3465,7 +3467,7 @@
       <c r="C68">
         <v>459</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="4">
         <v>10111</v>
       </c>
       <c r="E68">
@@ -3484,7 +3486,7 @@
       <c r="N68">
         <v>91</v>
       </c>
-      <c r="O68">
+      <c r="O68" s="4">
         <v>1001001</v>
       </c>
       <c r="P68">
@@ -3505,7 +3507,7 @@
       <c r="C69">
         <v>124</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="4">
         <v>11</v>
       </c>
       <c r="E69">
@@ -3524,7 +3526,7 @@
       <c r="N69">
         <v>72</v>
       </c>
-      <c r="O69">
+      <c r="O69" s="4">
         <v>1000</v>
       </c>
       <c r="P69">
@@ -3545,7 +3547,7 @@
       <c r="C70">
         <v>32</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="4">
         <v>100100</v>
       </c>
       <c r="E70">
@@ -3564,7 +3566,7 @@
       <c r="N70">
         <v>78</v>
       </c>
-      <c r="O70">
+      <c r="O70" s="4">
         <v>10011</v>
       </c>
       <c r="P70">
@@ -3585,7 +3587,7 @@
       <c r="C71">
         <v>407</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="4">
         <v>10100</v>
       </c>
       <c r="E71">
@@ -3604,7 +3606,7 @@
       <c r="N71">
         <v>86</v>
       </c>
-      <c r="O71">
+      <c r="O71" s="4">
         <v>101011</v>
       </c>
       <c r="P71">
@@ -3625,7 +3627,7 @@
       <c r="C72">
         <v>264</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="4">
         <v>111</v>
       </c>
       <c r="E72">
@@ -3644,7 +3646,7 @@
       <c r="N72">
         <v>73</v>
       </c>
-      <c r="O72">
+      <c r="O72" s="4">
         <v>1010</v>
       </c>
       <c r="P72">
@@ -3665,7 +3667,7 @@
       <c r="C73">
         <v>452</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="4">
         <v>10110</v>
       </c>
       <c r="E73">
@@ -3684,7 +3686,7 @@
       <c r="N73">
         <v>71</v>
       </c>
-      <c r="O73">
+      <c r="O73" s="4">
         <v>101</v>
       </c>
       <c r="P73">
@@ -3705,7 +3707,7 @@
       <c r="C74">
         <v>190</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="4">
         <v>100001</v>
       </c>
       <c r="E74">
@@ -3724,7 +3726,7 @@
       <c r="N74">
         <v>80</v>
       </c>
-      <c r="O74">
+      <c r="O74" s="4">
         <v>10101</v>
       </c>
       <c r="P74">
@@ -3745,7 +3747,7 @@
       <c r="C75">
         <v>30</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="4">
         <v>1000</v>
       </c>
       <c r="E75">
@@ -3764,7 +3766,7 @@
       <c r="N75">
         <v>111</v>
       </c>
-      <c r="O75">
+      <c r="O75" s="4">
         <v>1111111</v>
       </c>
       <c r="P75">
@@ -3785,7 +3787,7 @@
       <c r="C76">
         <v>26</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="4">
         <v>0</v>
       </c>
       <c r="E76">
@@ -3804,7 +3806,7 @@
       <c r="N76">
         <v>99</v>
       </c>
-      <c r="O76">
+      <c r="O76" s="4">
         <v>1101011</v>
       </c>
       <c r="P76">
@@ -3825,7 +3827,7 @@
       <c r="C77">
         <v>29</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="4">
         <v>110</v>
       </c>
       <c r="E77">
@@ -3844,7 +3846,7 @@
       <c r="N77">
         <v>108</v>
       </c>
-      <c r="O77">
+      <c r="O77" s="4">
         <v>1111100</v>
       </c>
       <c r="P77">
@@ -3865,7 +3867,7 @@
       <c r="C78">
         <v>12</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="4">
         <v>1001101001</v>
       </c>
       <c r="E78">
@@ -3884,7 +3886,7 @@
       <c r="N78">
         <v>78</v>
       </c>
-      <c r="O78">
+      <c r="O78" s="4">
         <v>10100</v>
       </c>
       <c r="P78">
@@ -3905,7 +3907,7 @@
       <c r="C79">
         <v>31</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="4">
         <v>100000</v>
       </c>
       <c r="E79">
@@ -3924,7 +3926,7 @@
       <c r="N79">
         <v>97</v>
       </c>
-      <c r="O79">
+      <c r="O79" s="4">
         <v>1100101</v>
       </c>
       <c r="P79">
@@ -3945,7 +3947,7 @@
       <c r="C80">
         <v>39</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="4">
         <v>10000000</v>
       </c>
       <c r="E80">
@@ -3964,7 +3966,7 @@
       <c r="N80">
         <v>70</v>
       </c>
-      <c r="O80">
+      <c r="O80" s="4">
         <v>100</v>
       </c>
       <c r="P80">
@@ -3985,7 +3987,7 @@
       <c r="C81">
         <v>2</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="4">
         <v>1000011000</v>
       </c>
       <c r="E81">
@@ -4004,7 +4006,7 @@
       <c r="N81">
         <v>97</v>
       </c>
-      <c r="O81">
+      <c r="O81" s="4">
         <v>1100111</v>
       </c>
       <c r="P81">
@@ -4025,7 +4027,7 @@
       <c r="C82">
         <v>39</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="4">
         <v>10000001</v>
       </c>
       <c r="E82">
@@ -4044,7 +4046,7 @@
       <c r="N82">
         <v>82</v>
       </c>
-      <c r="O82">
+      <c r="O82" s="4">
         <v>100001</v>
       </c>
       <c r="P82">
@@ -4065,7 +4067,7 @@
       <c r="N83">
         <v>92</v>
       </c>
-      <c r="O83">
+      <c r="O83" s="4">
         <v>1001111</v>
       </c>
       <c r="P83">
@@ -4086,7 +4088,7 @@
       <c r="N84">
         <v>91</v>
       </c>
-      <c r="O84">
+      <c r="O84" s="4">
         <v>1001100</v>
       </c>
       <c r="P84">
@@ -4126,7 +4128,7 @@
       <c r="N85">
         <v>73</v>
       </c>
-      <c r="O85">
+      <c r="O85" s="4">
         <v>1011</v>
       </c>
       <c r="P85">
@@ -4146,8 +4148,8 @@
         <v>11352</v>
       </c>
       <c r="D86" s="2">
-        <f>(82*2)+2</f>
-        <v>166</v>
+        <f>(82*2)+1</f>
+        <v>165</v>
       </c>
       <c r="E86" s="2">
         <f>_xlfn.CEILING.MATH(E87/8)</f>
@@ -4155,11 +4157,11 @@
       </c>
       <c r="F86" s="2">
         <f>_xlfn.CEILING.MATH(F87/8)</f>
-        <v>6395</v>
+        <v>6394</v>
       </c>
       <c r="G86" s="2">
         <f>F86/C86</f>
-        <v>0.56333685694150815</v>
+        <v>0.56324876673713886</v>
       </c>
       <c r="L86">
         <v>85</v>
@@ -4170,7 +4172,7 @@
       <c r="N86">
         <v>87</v>
       </c>
-      <c r="O86">
+      <c r="O86" s="4">
         <v>101111</v>
       </c>
       <c r="P86">
@@ -4191,7 +4193,7 @@
       </c>
       <c r="D87" s="2">
         <f>D86*8</f>
-        <v>1328</v>
+        <v>1320</v>
       </c>
       <c r="E87" s="2">
         <f>SUM($G$1:$G$82)</f>
@@ -4199,11 +4201,11 @@
       </c>
       <c r="F87" s="2">
         <f>E87+D87</f>
-        <v>51160</v>
+        <v>51152</v>
       </c>
       <c r="G87" s="2">
         <f>F87/C87</f>
-        <v>0.56333685694150815</v>
+        <v>0.56324876673713886</v>
       </c>
       <c r="L87">
         <v>86</v>
@@ -4214,7 +4216,7 @@
       <c r="N87">
         <v>87</v>
       </c>
-      <c r="O87">
+      <c r="O87" s="4">
         <v>110100</v>
       </c>
       <c r="P87">
@@ -4235,7 +4237,7 @@
       <c r="N88">
         <v>95</v>
       </c>
-      <c r="O88">
+      <c r="O88" s="4">
         <v>1011100</v>
       </c>
       <c r="P88">
@@ -4256,7 +4258,7 @@
       <c r="N89">
         <v>75</v>
       </c>
-      <c r="O89">
+      <c r="O89" s="4">
         <v>1111</v>
       </c>
       <c r="P89">
@@ -4277,7 +4279,7 @@
       <c r="N90">
         <v>83</v>
       </c>
-      <c r="O90">
+      <c r="O90" s="4">
         <v>100011</v>
       </c>
       <c r="P90">
@@ -4317,7 +4319,7 @@
       <c r="N91">
         <v>90</v>
       </c>
-      <c r="O91">
+      <c r="O91" s="4">
         <v>1000011</v>
       </c>
       <c r="P91">
@@ -4337,8 +4339,8 @@
         <v>11352</v>
       </c>
       <c r="D92" s="2">
-        <f>(127*2)+2</f>
-        <v>256</v>
+        <f>(127*2)+1</f>
+        <v>255</v>
       </c>
       <c r="E92" s="2">
         <f>_xlfn.CEILING.MATH(E93/8)</f>
@@ -4346,11 +4348,11 @@
       </c>
       <c r="F92" s="2">
         <f>_xlfn.CEILING.MATH(F93/8)</f>
-        <v>10176</v>
+        <v>10175</v>
       </c>
       <c r="G92" s="2">
         <f>F92/C92</f>
-        <v>0.89640591966173366</v>
+        <v>0.89631782945736438</v>
       </c>
       <c r="L92">
         <v>91</v>
@@ -4361,7 +4363,7 @@
       <c r="N92">
         <v>70</v>
       </c>
-      <c r="O92">
+      <c r="O92" s="4">
         <v>11</v>
       </c>
       <c r="P92">
@@ -4382,7 +4384,7 @@
       </c>
       <c r="D93" s="2">
         <f>D92*8</f>
-        <v>2048</v>
+        <v>2040</v>
       </c>
       <c r="E93" s="2">
         <f>SUM(R1:R127)</f>
@@ -4390,11 +4392,11 @@
       </c>
       <c r="F93" s="2">
         <f>E93+D93</f>
-        <v>81401</v>
+        <v>81393</v>
       </c>
       <c r="G93" s="2">
         <f>F93/C93</f>
-        <v>0.89632884073291053</v>
+        <v>0.89624075052854124</v>
       </c>
       <c r="L93">
         <v>92</v>
@@ -4405,7 +4407,7 @@
       <c r="N93">
         <v>94</v>
       </c>
-      <c r="O93">
+      <c r="O93" s="4">
         <v>1011001</v>
       </c>
       <c r="P93">
@@ -4426,7 +4428,7 @@
       <c r="N94">
         <v>86</v>
       </c>
-      <c r="O94">
+      <c r="O94" s="4">
         <v>101100</v>
       </c>
       <c r="P94">
@@ -4447,7 +4449,7 @@
       <c r="N95">
         <v>86</v>
       </c>
-      <c r="O95">
+      <c r="O95" s="4">
         <v>101101</v>
       </c>
       <c r="P95">
@@ -4468,7 +4470,7 @@
       <c r="N96">
         <v>105</v>
       </c>
-      <c r="O96">
+      <c r="O96" s="4">
         <v>1110110</v>
       </c>
       <c r="P96">
@@ -4489,7 +4491,7 @@
       <c r="N97">
         <v>89</v>
       </c>
-      <c r="O97">
+      <c r="O97" s="4">
         <v>111101</v>
       </c>
       <c r="P97">
@@ -4510,7 +4512,7 @@
       <c r="N98">
         <v>93</v>
       </c>
-      <c r="O98">
+      <c r="O98" s="4">
         <v>1010100</v>
       </c>
       <c r="P98">
@@ -4531,7 +4533,7 @@
       <c r="N99">
         <v>80</v>
       </c>
-      <c r="O99">
+      <c r="O99" s="4">
         <v>11001</v>
       </c>
       <c r="P99">
@@ -4552,7 +4554,7 @@
       <c r="N100">
         <v>108</v>
       </c>
-      <c r="O100">
+      <c r="O100" s="4">
         <v>1111101</v>
       </c>
       <c r="P100">
@@ -4573,7 +4575,7 @@
       <c r="N101">
         <v>87</v>
       </c>
-      <c r="O101">
+      <c r="O101" s="4">
         <v>110010</v>
       </c>
       <c r="P101">
@@ -4594,7 +4596,7 @@
       <c r="N102">
         <v>98</v>
       </c>
-      <c r="O102">
+      <c r="O102" s="4">
         <v>1101010</v>
       </c>
       <c r="P102">
@@ -4615,7 +4617,7 @@
       <c r="N103">
         <v>88</v>
       </c>
-      <c r="O103">
+      <c r="O103" s="4">
         <v>111001</v>
       </c>
       <c r="P103">
@@ -4636,7 +4638,7 @@
       <c r="N104">
         <v>111</v>
       </c>
-      <c r="O104">
+      <c r="O104" s="4">
         <v>0</v>
       </c>
       <c r="P104">
@@ -4657,7 +4659,7 @@
       <c r="N105">
         <v>100</v>
       </c>
-      <c r="O105">
+      <c r="O105" s="4">
         <v>1101110</v>
       </c>
       <c r="P105">
@@ -4678,7 +4680,7 @@
       <c r="N106">
         <v>90</v>
       </c>
-      <c r="O106">
+      <c r="O106" s="4">
         <v>1000010</v>
       </c>
       <c r="P106">
@@ -4699,7 +4701,7 @@
       <c r="N107">
         <v>91</v>
       </c>
-      <c r="O107">
+      <c r="O107" s="4">
         <v>1001010</v>
       </c>
       <c r="P107">
@@ -4720,7 +4722,7 @@
       <c r="N108">
         <v>95</v>
       </c>
-      <c r="O108">
+      <c r="O108" s="4">
         <v>1011101</v>
       </c>
       <c r="P108">
@@ -4741,7 +4743,7 @@
       <c r="N109">
         <v>72</v>
       </c>
-      <c r="O109">
+      <c r="O109" s="4">
         <v>1001</v>
       </c>
       <c r="P109">
@@ -4762,7 +4764,7 @@
       <c r="N110">
         <v>86</v>
       </c>
-      <c r="O110">
+      <c r="O110" s="4">
         <v>101110</v>
       </c>
       <c r="P110">
@@ -4783,7 +4785,7 @@
       <c r="N111">
         <v>80</v>
       </c>
-      <c r="O111">
+      <c r="O111" s="4">
         <v>11011</v>
       </c>
       <c r="P111">
@@ -4804,7 +4806,7 @@
       <c r="N112">
         <v>92</v>
       </c>
-      <c r="O112">
+      <c r="O112" s="4">
         <v>1010010</v>
       </c>
       <c r="P112">
@@ -4825,7 +4827,7 @@
       <c r="N113">
         <v>90</v>
       </c>
-      <c r="O113">
+      <c r="O113" s="4">
         <v>1000100</v>
       </c>
       <c r="P113">
@@ -4846,7 +4848,7 @@
       <c r="N114">
         <v>106</v>
       </c>
-      <c r="O114">
+      <c r="O114" s="4">
         <v>1110111</v>
       </c>
       <c r="P114">
@@ -4867,7 +4869,7 @@
       <c r="N115">
         <v>80</v>
       </c>
-      <c r="O115">
+      <c r="O115" s="4">
         <v>10110</v>
       </c>
       <c r="P115">
@@ -4888,7 +4890,7 @@
       <c r="N116">
         <v>108</v>
       </c>
-      <c r="O116">
+      <c r="O116" s="4">
         <v>1111110</v>
       </c>
       <c r="P116">
@@ -4909,7 +4911,7 @@
       <c r="N117">
         <v>97</v>
       </c>
-      <c r="O117">
+      <c r="O117" s="4">
         <v>1101000</v>
       </c>
       <c r="P117">
@@ -4930,7 +4932,7 @@
       <c r="N118">
         <v>96</v>
       </c>
-      <c r="O118">
+      <c r="O118" s="4">
         <v>1100000</v>
       </c>
       <c r="P118">
@@ -4951,7 +4953,7 @@
       <c r="N119">
         <v>87</v>
       </c>
-      <c r="O119">
+      <c r="O119" s="4">
         <v>110001</v>
       </c>
       <c r="P119">
@@ -4972,7 +4974,7 @@
       <c r="N120">
         <v>82</v>
       </c>
-      <c r="O120">
+      <c r="O120" s="4">
         <v>100010</v>
       </c>
       <c r="P120">
@@ -4993,7 +4995,7 @@
       <c r="N121">
         <v>81</v>
       </c>
-      <c r="O121">
+      <c r="O121" s="4">
         <v>11100</v>
       </c>
       <c r="P121">
@@ -5014,7 +5016,7 @@
       <c r="N122">
         <v>83</v>
       </c>
-      <c r="O122">
+      <c r="O122" s="4">
         <v>100101</v>
       </c>
       <c r="P122">
@@ -5035,7 +5037,7 @@
       <c r="N123">
         <v>92</v>
       </c>
-      <c r="O123">
+      <c r="O123" s="4">
         <v>1010001</v>
       </c>
       <c r="P123">
@@ -5056,7 +5058,7 @@
       <c r="N124">
         <v>100</v>
       </c>
-      <c r="O124">
+      <c r="O124" s="4">
         <v>1101100</v>
       </c>
       <c r="P124">
@@ -5077,7 +5079,7 @@
       <c r="N125">
         <v>90</v>
       </c>
-      <c r="O125">
+      <c r="O125" s="4">
         <v>1000101</v>
       </c>
       <c r="P125">
@@ -5098,7 +5100,7 @@
       <c r="N126">
         <v>68</v>
       </c>
-      <c r="O126">
+      <c r="O126" s="4">
         <v>10</v>
       </c>
       <c r="P126">
@@ -5119,7 +5121,7 @@
       <c r="N127">
         <v>101</v>
       </c>
-      <c r="O127">
+      <c r="O127" s="4">
         <v>1101111</v>
       </c>
       <c r="P127">

</xml_diff>